<commit_message>
rs data onboarding tracking
</commit_message>
<xml_diff>
--- a/data/raw/FLDEP.xlsx
+++ b/data/raw/FLDEP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bearden_M\Desktop\Piney Point\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\piney-point\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D63EE1C-3B7E-4DA2-819A-364C4BE57E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703AC0DB-0EBE-43F8-8B73-2DC19E000E38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{66163D4F-7B67-4B0E-A1E8-9D35ACF0F835}"/>
+    <workbookView xWindow="35370" yWindow="2355" windowWidth="19905" windowHeight="9600" xr2:uid="{66163D4F-7B67-4B0E-A1E8-9D35ACF0F835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Latitude</t>
   </si>
@@ -114,6 +106,30 @@
   </si>
   <si>
     <t>Manatee County - 449</t>
+  </si>
+  <si>
+    <t>Piney 4</t>
+  </si>
+  <si>
+    <t>Piney 1</t>
+  </si>
+  <si>
+    <t>Piney 2</t>
+  </si>
+  <si>
+    <t>Piney 5</t>
+  </si>
+  <si>
+    <t>P Port 1</t>
+  </si>
+  <si>
+    <t>P Port 2</t>
+  </si>
+  <si>
+    <t>P Port 3</t>
+  </si>
+  <si>
+    <t>P Port 4</t>
   </si>
 </sst>
 </file>
@@ -471,22 +487,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B6D0C8-24CB-48A0-B72C-742B2F39B409}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>27.6434</v>
       </c>
@@ -520,7 +536,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>27.626000000000001</v>
       </c>
@@ -537,7 +553,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>27.662500000000001</v>
       </c>
@@ -554,7 +570,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>27.612974999999999</v>
       </c>
@@ -571,7 +587,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>27.605986000000001</v>
       </c>
@@ -588,7 +604,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>27.572583000000002</v>
       </c>
@@ -605,7 +621,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>27.576508</v>
       </c>
@@ -622,7 +638,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>27.543099999999999</v>
       </c>
@@ -639,7 +655,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>27.552008000000001</v>
       </c>
@@ -656,7 +672,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>27.533000000000001</v>
       </c>
@@ -673,7 +689,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>27.545808000000001</v>
       </c>
@@ -688,6 +704,94 @@
       </c>
       <c r="E12">
         <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>27.6358</v>
+      </c>
+      <c r="B13">
+        <v>-82.565299999999993</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>27.64742</v>
+      </c>
+      <c r="B14">
+        <v>-82.565160000000006</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>27.649480000000001</v>
+      </c>
+      <c r="B15">
+        <v>-82.578450000000004</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>27.628520000000002</v>
+      </c>
+      <c r="B16">
+        <v>-82.591930000000005</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>27.634879999999999</v>
+      </c>
+      <c r="B17">
+        <v>-82.563190000000006</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>27.631049999999998</v>
+      </c>
+      <c r="B18">
+        <v>-82.557590000000005</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>27.631409999999999</v>
+      </c>
+      <c r="B19">
+        <v>-82.544269999999997</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>27.645399999999999</v>
+      </c>
+      <c r="B20">
+        <v>-82.536950000000004</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fldep 20210408 data dump
</commit_message>
<xml_diff>
--- a/data/raw/FLDEP.xlsx
+++ b/data/raw/FLDEP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\piney-point\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703AC0DB-0EBE-43F8-8B73-2DC19E000E38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EE5654-0935-4450-8436-854AD0E2663A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35370" yWindow="2355" windowWidth="19905" windowHeight="9600" xr2:uid="{66163D4F-7B67-4B0E-A1E8-9D35ACF0F835}"/>
+    <workbookView xWindow="36015" yWindow="1995" windowWidth="19905" windowHeight="12030" xr2:uid="{66163D4F-7B67-4B0E-A1E8-9D35ACF0F835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Latitude</t>
   </si>
@@ -130,6 +130,27 @@
   </si>
   <si>
     <t>P Port 4</t>
+  </si>
+  <si>
+    <t>Piney 22</t>
+  </si>
+  <si>
+    <t>Piney 18</t>
+  </si>
+  <si>
+    <t>Piney 20</t>
+  </si>
+  <si>
+    <t>Piney 19</t>
+  </si>
+  <si>
+    <t>Piney 21</t>
+  </si>
+  <si>
+    <t>Piney 23</t>
+  </si>
+  <si>
+    <t>Piney 17</t>
   </si>
 </sst>
 </file>
@@ -487,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B6D0C8-24CB-48A0-B72C-742B2F39B409}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,88 +541,58 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>27.6434</v>
-      </c>
-      <c r="B2" s="2">
-        <v>-82.577100000000002</v>
+      <c r="A2">
+        <v>27.634879999999999</v>
+      </c>
+      <c r="B2">
+        <v>-82.563190000000006</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>165</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>27.626000000000001</v>
-      </c>
-      <c r="B3" s="2">
-        <v>-82.591499999999996</v>
+      <c r="A3">
+        <v>27.631049999999998</v>
+      </c>
+      <c r="B3">
+        <v>-82.557590000000005</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>165</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>27.662500000000001</v>
+        <v>27.631409999999999</v>
       </c>
       <c r="B4">
-        <v>-82.563903999999994</v>
+        <v>-82.544269999999997</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>165</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>27.612974999999999</v>
+        <v>27.645399999999999</v>
       </c>
       <c r="B5">
-        <v>-82.577641999999997</v>
+        <v>-82.536950000000004</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>165</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>27.605986000000001</v>
+        <v>27.64742</v>
       </c>
       <c r="B6">
-        <v>-82.601167000000004</v>
+        <v>-82.565160000000006</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>165</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -708,35 +699,41 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>27.6358</v>
+        <v>27.649480000000001</v>
       </c>
       <c r="B13">
-        <v>-82.565299999999993</v>
+        <v>-82.578450000000004</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>27.64742</v>
-      </c>
-      <c r="B14">
-        <v>-82.565160000000006</v>
+      <c r="A14" s="1">
+        <v>27.6434</v>
+      </c>
+      <c r="B14" s="2">
+        <v>-82.577100000000002</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>27.649480000000001</v>
+        <v>27.6358</v>
       </c>
       <c r="B15">
-        <v>-82.578450000000004</v>
+        <v>-82.565299999999993</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -750,51 +747,155 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>27.634879999999999</v>
-      </c>
-      <c r="B17">
-        <v>-82.563190000000006</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>27.626000000000001</v>
+      </c>
+      <c r="B17" s="2">
+        <v>-82.591499999999996</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>27.631049999999998</v>
+        <v>27.662500000000001</v>
       </c>
       <c r="B18">
-        <v>-82.557590000000005</v>
+        <v>-82.563903999999994</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>27.631409999999999</v>
+        <v>27.612974999999999</v>
       </c>
       <c r="B19">
-        <v>-82.544269999999997</v>
+        <v>-82.577641999999997</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>27.645399999999999</v>
+        <v>27.605986000000001</v>
       </c>
       <c r="B20">
-        <v>-82.536950000000004</v>
+        <v>-82.601167000000004</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>27.781299000000001</v>
+      </c>
+      <c r="B21">
+        <v>-82.474100000000007</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>27.682528999999999</v>
+      </c>
+      <c r="B22">
+        <v>-82.496769999999998</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>27.728999999999999</v>
+      </c>
+      <c r="B23">
+        <v>-82.498699999999999</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>27.723801000000002</v>
+      </c>
+      <c r="B24">
+        <v>-82.533799999999999</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>27.777999999999999</v>
+      </c>
+      <c r="B25">
+        <v>-82.520300000000006</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>27.776399999999999</v>
+      </c>
+      <c r="B26">
+        <v>-82.438730000000007</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>27.693398999999999</v>
+      </c>
+      <c r="B27">
+        <v>-82.555899999999994</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E20">
+    <sortCondition ref="C1:C20"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated fldep 2022 data, removing dup epchc data
</commit_message>
<xml_diff>
--- a/data/raw/FLDEP.xlsx
+++ b/data/raw/FLDEP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\piney-point\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EE5654-0935-4450-8436-854AD0E2663A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D71696F-2FEA-4DE4-A1BE-8DE073A06716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36015" yWindow="1995" windowWidth="19905" windowHeight="12030" xr2:uid="{66163D4F-7B67-4B0E-A1E8-9D35ACF0F835}"/>
+    <workbookView xWindow="32730" yWindow="1995" windowWidth="20430" windowHeight="11640" xr2:uid="{66163D4F-7B67-4B0E-A1E8-9D35ACF0F835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Latitude</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Piney 17</t>
+  </si>
+  <si>
+    <t>Piney 24</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -182,17 +185,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B6D0C8-24CB-48A0-B72C-742B2F39B409}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,7 +902,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>27.693398999999999</v>
       </c>
@@ -890,6 +911,17 @@
       </c>
       <c r="C27" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>27.626000000000001</v>
+      </c>
+      <c r="B28" s="3">
+        <v>-82.591499999999996</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -897,5 +929,6 @@
     <sortCondition ref="C1:C20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>